<commit_message>
add new season file
</commit_message>
<xml_diff>
--- a/data/season/current_season/Triathlon Season.xlsx
+++ b/data/season/current_season/Triathlon Season.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,7 +427,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>south coast</v>
+        <v>South Coast League</v>
       </c>
       <c r="B2" t="str">
         <v>1</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>south coast</v>
+        <v>South Coast League</v>
       </c>
       <c r="B3" t="str">
         <v>2</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>south coast</v>
+        <v>South Coast League</v>
       </c>
       <c r="B4" t="str">
         <v>3</v>
@@ -488,7 +488,7 @@
         <v xml:space="preserve">Sprint,  Standard </v>
       </c>
       <c r="F4" t="str">
-        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
       </c>
       <c r="G4" t="str">
         <v>Eurocoast Triathlon Club</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>south coast</v>
+        <v>South Coast League</v>
       </c>
       <c r="B5" t="str">
         <v>4</v>
@@ -508,7 +508,7 @@
         <v>no</v>
       </c>
       <c r="E5" t="str">
-        <v>Super Sprint, Sprint, Classic and Ultimate</v>
+        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
       </c>
       <c r="F5" t="str">
         <v>Ultra and Aquabike</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>south coast</v>
+        <v>South Coast League</v>
       </c>
       <c r="B6" t="str">
         <v>5</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="B7" t="str">
         <v>1</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="B8" t="str">
         <v>2</v>
@@ -577,7 +577,7 @@
         <v>Sprint</v>
       </c>
       <c r="F8" t="str">
-        <v>Super Sprint, Aquathlon, Teams</v>
+        <v>Super Sprint, Aquathon, Teams</v>
       </c>
       <c r="G8" t="str">
         <v>Yamba Multisport</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="B9" t="str">
         <v>3</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="B10" t="str">
         <v>4</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="B11" t="str">
         <v>5</v>
@@ -646,7 +646,7 @@
         <v>Sprint and Standard</v>
       </c>
       <c r="F11" t="str">
-        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
       </c>
       <c r="G11" t="str">
         <v>Grafton Triathlon Club</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="B12" t="str">
         <v>6</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>North Coast</v>
+        <v>North Coast League</v>
       </c>
       <c r="G13" t="str">
         <v>Port Macquarie Triathlon Club</v>
@@ -697,10 +697,10 @@
         <v>no</v>
       </c>
       <c r="E14" t="str">
-        <v>ironman 70.3, Sprint</v>
+        <v>Ironman 70.3 and Sprint</v>
       </c>
       <c r="F14" t="str">
-        <v>Aquabike</v>
+        <v>n/a</v>
       </c>
       <c r="G14" t="str">
         <v>Cronulla Triathlon Club</v>
@@ -766,10 +766,10 @@
         <v>no</v>
       </c>
       <c r="E17" t="str">
-        <v>Long Aquathlon</v>
+        <v>Long Aqua</v>
       </c>
       <c r="F17" t="str">
-        <v>Super Sprint Aquathlon</v>
+        <v>Short Aqua</v>
       </c>
       <c r="G17" t="str">
         <v>Manly Vipers Triathlon Club</v>
@@ -789,7 +789,7 @@
         <v>no</v>
       </c>
       <c r="E18" t="str">
-        <v>Enticer, Sprint</v>
+        <v>Super Sprint, Sprint</v>
       </c>
       <c r="F18" t="str">
         <v>n/a</v>
@@ -812,7 +812,7 @@
         <v>no</v>
       </c>
       <c r="E19" t="str">
-        <v>Super Sprint, Sprint, Classic and Ultimate</v>
+        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
       </c>
       <c r="F19" t="str">
         <v>Aquabike</v>
@@ -882,10 +882,10 @@
         <v>no</v>
       </c>
       <c r="E24" t="str">
-        <v>ironman 70.3, Sprint</v>
+        <v>Ironman 70.3 and Sprint</v>
       </c>
       <c r="F24" t="str">
-        <v>Aquabike</v>
+        <v>n/a</v>
       </c>
       <c r="G24" t="str">
         <v>Moore Performance Triathlon Club</v>
@@ -905,7 +905,7 @@
         <v>yes</v>
       </c>
       <c r="E25" t="str">
-        <v>Standard, Standard Aquabike</v>
+        <v>Standard, Aquabike</v>
       </c>
       <c r="F25" t="str">
         <v>Sprint</v>
@@ -951,10 +951,10 @@
         <v>no</v>
       </c>
       <c r="E27" t="str">
-        <v>Long Aquathlon</v>
+        <v>Long Aqua</v>
       </c>
       <c r="F27" t="str">
-        <v>Super Sprint Aquathlon</v>
+        <v>Short Aqua</v>
       </c>
       <c r="G27" t="str">
         <v>FilOz Triathlon Club</v>
@@ -974,7 +974,7 @@
         <v>no</v>
       </c>
       <c r="E28" t="str">
-        <v>Enticer, Sprint</v>
+        <v>Super Sprint, Sprint</v>
       </c>
       <c r="F28" t="str">
         <v>n/a</v>
@@ -997,7 +997,7 @@
         <v>no</v>
       </c>
       <c r="E29" t="str">
-        <v>Super Sprint, Sprint, Classic and Ultimate</v>
+        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
       </c>
       <c r="F29" t="str">
         <v>Aquabike</v>
@@ -1020,7 +1020,7 @@
         <v>no</v>
       </c>
       <c r="E30" t="str">
-        <v>Sprint, Olympic</v>
+        <v>Sprint, Standard</v>
       </c>
       <c r="F30" t="str">
         <v>Super Sprint, Aquabike</v>
@@ -1077,13 +1077,13 @@
         <v>1</v>
       </c>
       <c r="C36" t="str">
-        <v>Stockton Island</v>
+        <v>Sparke Helmore Triathlon</v>
       </c>
       <c r="D36" t="str">
         <v>No</v>
       </c>
       <c r="E36" t="str">
-        <v>Sprint, Standard</v>
+        <v>Sprint and Standard</v>
       </c>
       <c r="F36" t="str">
         <v>N/A</v>
@@ -1100,39 +1100,434 @@
         <v>2</v>
       </c>
       <c r="C37" t="str">
-        <v>Sparke Helmore Triathlon</v>
+        <v>Hawks Nest Triathlon</v>
       </c>
       <c r="D37" t="str">
         <v>No</v>
       </c>
       <c r="E37" t="str">
-        <v>Sprint</v>
+        <v>Sprint, Standard</v>
       </c>
       <c r="F37" t="str">
-        <v>Super Sprint</v>
+        <v>Super Sprint, Aquabike</v>
       </c>
       <c r="G37" t="str">
         <v>Forster Triathlon Club</v>
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="str">
+        <v>Hunter League</v>
+      </c>
+      <c r="B38" t="str">
+        <v>3</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Singleton Triathlon</v>
+      </c>
+      <c r="D38" t="str">
+        <v>No</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Sprint</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Super Sprint</v>
+      </c>
       <c r="G38" t="str">
         <v>Singleton Triathlon Club</v>
       </c>
     </row>
     <row r="39">
+      <c r="A39" t="str">
+        <v>Hunter League</v>
+      </c>
+      <c r="B39" t="str">
+        <v>4</v>
+      </c>
+      <c r="C39" t="str">
+        <v>CCTRI Club Race</v>
+      </c>
+      <c r="D39" t="str">
+        <v>No</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Sprint</v>
+      </c>
+      <c r="F39" t="str">
+        <v>Super Sprint</v>
+      </c>
       <c r="G39" t="str">
         <v>Maitland Triathlon Club</v>
       </c>
     </row>
     <row r="40">
+      <c r="A40" t="str">
+        <v>Hunter League</v>
+      </c>
+      <c r="B40" t="str">
+        <v>5</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Island Triathlon</v>
+      </c>
+      <c r="D40" t="str">
+        <v>No</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Super Sprint, Sprint, Standard, Aquabike</v>
+      </c>
+      <c r="F40" t="str">
+        <v>n/a</v>
+      </c>
       <c r="G40" t="str">
         <v>Newcastle Traithlon Club</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Hunter League</v>
+      </c>
+      <c r="B41" t="str">
+        <v>6</v>
+      </c>
+      <c r="C41" t="str">
+        <v>NSW Triathlon Club Champs (Double Points)</v>
+      </c>
+      <c r="D41" t="str">
+        <v>yes</v>
+      </c>
+      <c r="E41" t="str">
+        <v xml:space="preserve">Sprint, Standard </v>
+      </c>
+      <c r="F41" t="str">
+        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Hunter League</v>
+      </c>
+      <c r="B42" t="str">
+        <v>7</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Lake Macquarie Triathlon Festival</v>
+      </c>
+      <c r="D42" t="str">
+        <v>No</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Sprint and Standard</v>
+      </c>
+      <c r="F42" t="str">
+        <v>Super Sprint</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Central West League</v>
+      </c>
+      <c r="B43" t="str">
+        <v>1</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Mudgee Triathlon Club</v>
+      </c>
+      <c r="D43" t="str">
+        <v>No</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Club Distance</v>
+      </c>
+      <c r="F43" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G43" t="str">
+        <v>Mudgee Triathlon Club</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Central West League</v>
+      </c>
+      <c r="B44" t="str">
+        <v>2</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Bathurst  Triathlon Club</v>
+      </c>
+      <c r="D44" t="str">
+        <v>No</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Club Distance</v>
+      </c>
+      <c r="F44" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G44" t="str">
+        <v>Bathurst  Triathlon Club</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Central West League</v>
+      </c>
+      <c r="B45" t="str">
+        <v>3</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Orange Triathlon Club</v>
+      </c>
+      <c r="D45" t="str">
+        <v>No</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Club Distance</v>
+      </c>
+      <c r="F45" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Orange Triathlon Club</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Central West League</v>
+      </c>
+      <c r="B46" t="str">
+        <v>4</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Dubbo Triathlon Club</v>
+      </c>
+      <c r="D46" t="str">
+        <v>No</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Club Distance</v>
+      </c>
+      <c r="F46" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G46" t="str">
+        <v>Dubbo Triathlon Club</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="G47" t="str">
+        <v>Cowra Triathlon Club</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>New England League</v>
+      </c>
+      <c r="B48" t="str">
+        <v>1</v>
+      </c>
+      <c r="C48" t="str">
+        <v xml:space="preserve">Scone Club Race </v>
+      </c>
+      <c r="D48" t="str">
+        <v>No</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Sprint and Super Sprint</v>
+      </c>
+      <c r="F48" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G48" t="str">
+        <v>Scone Triathlon Club</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>New England League</v>
+      </c>
+      <c r="B49" t="str">
+        <v>2</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Tamworth Club Race</v>
+      </c>
+      <c r="D49" t="str">
+        <v>No</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Club Distance</v>
+      </c>
+      <c r="F49" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G49" t="str">
+        <v>Armidale Triathlon Club</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>New England League</v>
+      </c>
+      <c r="B50" t="str">
+        <v>3</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Armidale Club Race</v>
+      </c>
+      <c r="D50" t="str">
+        <v>No</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Club Distance</v>
+      </c>
+      <c r="F50" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G50" t="str">
+        <v>Gunnedah Triathlon Club</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>New England League</v>
+      </c>
+      <c r="B51" t="str">
+        <v>4</v>
+      </c>
+      <c r="C51" t="str">
+        <v>NSW Triathlon Club Champs</v>
+      </c>
+      <c r="D51" t="str">
+        <v>yes</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Sprint, Standard</v>
+      </c>
+      <c r="F51" t="str">
+        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+      </c>
+      <c r="G51" t="str">
+        <v>Tamworth Triathlon Club</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Hume League</v>
+      </c>
+      <c r="B52" t="str">
+        <v>1</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Challenge Canberra</v>
+      </c>
+      <c r="D52" t="str">
+        <v>No</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Ironman 70.3, Aquabike 70.3, Standard, Aquabike, Sprint</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Super Sprint</v>
+      </c>
+      <c r="G52" t="str">
+        <v>Yass Valley Triathlon Club</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Hume League</v>
+      </c>
+      <c r="B53" t="str">
+        <v>2</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Jackie Fairweather Triathlon</v>
+      </c>
+      <c r="D53" t="str">
+        <v>No</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Sprint</v>
+      </c>
+      <c r="F53" t="str">
+        <v>Super Sprint</v>
+      </c>
+      <c r="G53" t="str">
+        <v>Goulburn Triathlon Club</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Hume League</v>
+      </c>
+      <c r="B54" t="str">
+        <v>3</v>
+      </c>
+      <c r="C54" t="str">
+        <v>MMJ Aquathlon</v>
+      </c>
+      <c r="D54" t="str">
+        <v>No</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Long Aqua</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Short Aqua, Mini Aqua</v>
+      </c>
+      <c r="G54" t="str">
+        <v>Leeton Triathlon Club</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Hume League</v>
+      </c>
+      <c r="B55" t="str">
+        <v>4</v>
+      </c>
+      <c r="C55" t="str">
+        <v>NSW Triathlon Club Champs (Double Points)</v>
+      </c>
+      <c r="D55" t="str">
+        <v>yes</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Sprint, Standard</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+      </c>
+      <c r="G55" t="str">
+        <v>Wagga TrIathlon Club</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Hume League</v>
+      </c>
+      <c r="B56" t="str">
+        <v>5</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Big Husky</v>
+      </c>
+      <c r="D56" t="str">
+        <v>No</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Aquabike</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G40"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G56"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding rounding function and updating participation points logic; update Triathlon Season.xlsx
</commit_message>
<xml_diff>
--- a/data/season/current_season/Triathlon Season.xlsx
+++ b/data/season/current_season/Triathlon Season.xlsx
@@ -427,7 +427,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>South Coast League</v>
+        <v>south coast league</v>
       </c>
       <c r="B2" t="str">
         <v>1</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>South Coast League</v>
+        <v>south coast league</v>
       </c>
       <c r="B3" t="str">
         <v>2</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>South Coast League</v>
+        <v>south coast league</v>
       </c>
       <c r="B4" t="str">
         <v>3</v>
@@ -488,7 +488,7 @@
         <v xml:space="preserve">Sprint,  Standard </v>
       </c>
       <c r="F4" t="str">
-        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
       </c>
       <c r="G4" t="str">
         <v>Eurocoast Triathlon Club</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>South Coast League</v>
+        <v>south coast league</v>
       </c>
       <c r="B5" t="str">
         <v>4</v>
@@ -508,7 +508,7 @@
         <v>no</v>
       </c>
       <c r="E5" t="str">
-        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
+        <v>Super Sprint, Sprint, Classic and Ultimate</v>
       </c>
       <c r="F5" t="str">
         <v>Ultra and Aquabike</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>South Coast League</v>
+        <v>south coast league</v>
       </c>
       <c r="B6" t="str">
         <v>5</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="B7" t="str">
         <v>1</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="B8" t="str">
         <v>2</v>
@@ -577,7 +577,7 @@
         <v>Sprint</v>
       </c>
       <c r="F8" t="str">
-        <v>Super Sprint, Aquathon, Teams</v>
+        <v>Super Sprint, Aquathlon, Teams</v>
       </c>
       <c r="G8" t="str">
         <v>Yamba Multisport</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="B9" t="str">
         <v>3</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="B10" t="str">
         <v>4</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="B11" t="str">
         <v>5</v>
@@ -646,7 +646,7 @@
         <v>Sprint and Standard</v>
       </c>
       <c r="F11" t="str">
-        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
       </c>
       <c r="G11" t="str">
         <v>Grafton Triathlon Club</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="B12" t="str">
         <v>6</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>North Coast League</v>
+        <v>North Coast league</v>
       </c>
       <c r="G13" t="str">
         <v>Port Macquarie Triathlon Club</v>
@@ -697,10 +697,10 @@
         <v>no</v>
       </c>
       <c r="E14" t="str">
-        <v>Ironman 70.3 and Sprint</v>
+        <v>70.3 and Sprint</v>
       </c>
       <c r="F14" t="str">
-        <v>n/a</v>
+        <v>Aquabike</v>
       </c>
       <c r="G14" t="str">
         <v>Cronulla Triathlon Club</v>
@@ -714,16 +714,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="str">
-        <v>NSW Triathlon Club Champs</v>
+        <v>Sparke Helmore Triathlon</v>
       </c>
       <c r="D15" t="str">
-        <v>yes</v>
+        <v>No</v>
       </c>
       <c r="E15" t="str">
-        <v>Standard, Aquabike</v>
+        <v>Sprint</v>
       </c>
       <c r="F15" t="str">
-        <v>Sprint</v>
+        <v>Super Sprint, Aquabike</v>
       </c>
       <c r="G15" t="str">
         <v>Warringah Triathlon Club</v>
@@ -766,10 +766,10 @@
         <v>no</v>
       </c>
       <c r="E17" t="str">
-        <v>Long Aqua</v>
+        <v>Long Aquathlon</v>
       </c>
       <c r="F17" t="str">
-        <v>Short Aqua</v>
+        <v>Super Sprint Aquathlon</v>
       </c>
       <c r="G17" t="str">
         <v>Manly Vipers Triathlon Club</v>
@@ -783,16 +783,16 @@
         <v>5</v>
       </c>
       <c r="C18" t="str">
-        <v>Sparke Helmore Triathlon</v>
+        <v>NSW Triathlon Club Champs</v>
       </c>
       <c r="D18" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="E18" t="str">
-        <v>Super Sprint, Sprint</v>
+        <v xml:space="preserve">Sprint,  Standard </v>
       </c>
       <c r="F18" t="str">
-        <v>n/a</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
       </c>
       <c r="G18" t="str">
         <v>Concord Triathlon Club</v>
@@ -812,7 +812,7 @@
         <v>no</v>
       </c>
       <c r="E19" t="str">
-        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
+        <v>Super Sprint, Sprint, Classic and Ultimate</v>
       </c>
       <c r="F19" t="str">
         <v>Aquabike</v>
@@ -882,10 +882,10 @@
         <v>no</v>
       </c>
       <c r="E24" t="str">
-        <v>Ironman 70.3 and Sprint</v>
+        <v>70.3 and Sprint</v>
       </c>
       <c r="F24" t="str">
-        <v>n/a</v>
+        <v>Aquabike</v>
       </c>
       <c r="G24" t="str">
         <v>Moore Performance Triathlon Club</v>
@@ -899,16 +899,16 @@
         <v>2</v>
       </c>
       <c r="C25" t="str">
-        <v>NSW Triathlon Club Champs</v>
+        <v>Sparke Helmore Triathlon</v>
       </c>
       <c r="D25" t="str">
-        <v>yes</v>
+        <v>No</v>
       </c>
       <c r="E25" t="str">
-        <v>Standard, Aquabike</v>
+        <v>Sprint</v>
       </c>
       <c r="F25" t="str">
-        <v>Sprint</v>
+        <v>Super Sprint, Aquabike</v>
       </c>
       <c r="G25" t="str">
         <v>TriMob</v>
@@ -951,10 +951,10 @@
         <v>no</v>
       </c>
       <c r="E27" t="str">
-        <v>Long Aqua</v>
+        <v>Long Aquathlon</v>
       </c>
       <c r="F27" t="str">
-        <v>Short Aqua</v>
+        <v>Super Sprint Aquathlon</v>
       </c>
       <c r="G27" t="str">
         <v>FilOz Triathlon Club</v>
@@ -968,16 +968,16 @@
         <v>5</v>
       </c>
       <c r="C28" t="str">
-        <v>Sparke Helmore Triathlon</v>
+        <v>NSW Triathlon Club Champs</v>
       </c>
       <c r="D28" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="E28" t="str">
-        <v>Super Sprint, Sprint</v>
+        <v xml:space="preserve">Sprint,  Standard </v>
       </c>
       <c r="F28" t="str">
-        <v>n/a</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
       </c>
       <c r="G28" t="str">
         <v>Hills Triathlon Club</v>
@@ -997,7 +997,7 @@
         <v>no</v>
       </c>
       <c r="E29" t="str">
-        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
+        <v>Super Sprint, Sprint, Classic and Ultimate</v>
       </c>
       <c r="F29" t="str">
         <v>Aquabike</v>
@@ -1020,7 +1020,7 @@
         <v>no</v>
       </c>
       <c r="E30" t="str">
-        <v>Sprint, Standard</v>
+        <v>Sprint, Olympic</v>
       </c>
       <c r="F30" t="str">
         <v>Super Sprint, Aquabike</v>
@@ -1083,13 +1083,13 @@
         <v>No</v>
       </c>
       <c r="E36" t="str">
-        <v>Sprint and Standard</v>
+        <v>Sprint</v>
       </c>
       <c r="F36" t="str">
-        <v>N/A</v>
+        <v>Super Sprint, Aquabike</v>
       </c>
       <c r="G36" t="str">
-        <v>Central Coast Triathlon Club</v>
+        <v>Forster Triathlon Club</v>
       </c>
     </row>
     <row r="37">
@@ -1109,10 +1109,10 @@
         <v>Sprint, Standard</v>
       </c>
       <c r="F37" t="str">
-        <v>Super Sprint, Aquabike</v>
+        <v>Super Sprint, Standard Aquabike</v>
       </c>
       <c r="G37" t="str">
-        <v>Forster Triathlon Club</v>
+        <v>Newcastle Triathlon Club</v>
       </c>
     </row>
     <row r="38">
@@ -1135,7 +1135,7 @@
         <v>Super Sprint</v>
       </c>
       <c r="G38" t="str">
-        <v>Singleton Triathlon Club</v>
+        <v>Central Coast Triathlon Club</v>
       </c>
     </row>
     <row r="39">
@@ -1158,7 +1158,7 @@
         <v>Super Sprint</v>
       </c>
       <c r="G39" t="str">
-        <v>Maitland Triathlon Club</v>
+        <v>Singleton Triathlon Club</v>
       </c>
     </row>
     <row r="40">
@@ -1181,7 +1181,7 @@
         <v>n/a</v>
       </c>
       <c r="G40" t="str">
-        <v>Newcastle Traithlon Club</v>
+        <v>Maitland Triathlon Club</v>
       </c>
     </row>
     <row r="41">
@@ -1192,16 +1192,19 @@
         <v>6</v>
       </c>
       <c r="C41" t="str">
-        <v>NSW Triathlon Club Champs (Double Points)</v>
+        <v>NSW Triathlon Club Champs</v>
       </c>
       <c r="D41" t="str">
         <v>yes</v>
       </c>
       <c r="E41" t="str">
-        <v xml:space="preserve">Sprint, Standard </v>
+        <v xml:space="preserve">Sprint,  Standard </v>
       </c>
       <c r="F41" t="str">
-        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
+      </c>
+      <c r="G41" t="str">
+        <v>Tomaree Triathlon Club</v>
       </c>
     </row>
     <row r="42">
@@ -1407,7 +1410,7 @@
         <v>Sprint, Standard</v>
       </c>
       <c r="F51" t="str">
-        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
       </c>
       <c r="G51" t="str">
         <v>Tamworth Triathlon Club</v>
@@ -1427,7 +1430,7 @@
         <v>No</v>
       </c>
       <c r="E52" t="str">
-        <v>Ironman 70.3, Aquabike 70.3, Standard, Aquabike, Sprint</v>
+        <v>70.3, 70.3 Aquabike, Standard, Standard Aquabike, Sprint</v>
       </c>
       <c r="F52" t="str">
         <v>Super Sprint</v>
@@ -1473,7 +1476,7 @@
         <v>No</v>
       </c>
       <c r="E54" t="str">
-        <v>Long Aqua</v>
+        <v>Long Aquathlon</v>
       </c>
       <c r="F54" t="str">
         <v>Short Aqua, Mini Aqua</v>
@@ -1499,7 +1502,7 @@
         <v>Sprint, Standard</v>
       </c>
       <c r="F55" t="str">
-        <v>Sprint Aquabike, Aquabike, Super Sprint</v>
+        <v>Sprint Aquabike, Standard Aquabike, Super Sprint</v>
       </c>
       <c r="G55" t="str">
         <v>Wagga TrIathlon Club</v>
@@ -1519,7 +1522,7 @@
         <v>No</v>
       </c>
       <c r="E56" t="str">
-        <v>Super Sprint, Sprint, Classic and Ironman 70.3</v>
+        <v>Super Sprint, Sprint, Classic and Ultimate</v>
       </c>
       <c r="F56" t="str">
         <v>Aquabike</v>

</xml_diff>